<commit_message>
Work on config parsing
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colten\Dropbox\_SCHOOL\ECE_412_Capstone1\sense_platform\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9465"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -78,9 +83,6 @@
     <t>Micro USB, type B, male</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Accelerometer</t>
   </si>
   <si>
@@ -271,6 +273,9 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total: </t>
   </si>
 </sst>
 </file>
@@ -313,7 +318,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -336,12 +341,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -351,18 +369,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -374,6 +396,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -422,7 +447,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -457,7 +482,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -669,7 +694,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,15 +703,15 @@
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="5" max="5" width="59" customWidth="1"/>
     <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="75.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -706,46 +731,46 @@
         <v>3</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>32</v>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="8">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="10">
+      <c r="F2" s="7">
+        <v>6</v>
+      </c>
+      <c r="G2" s="9">
         <v>7.55</v>
       </c>
-      <c r="I2" s="10">
-        <f t="shared" ref="I2:I16" si="0">F2*H2</f>
+      <c r="H2" s="9">
+        <f>F2*G2</f>
         <v>45.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="I2" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -761,18 +786,18 @@
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="7">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5">
+        <v>9.01</v>
+      </c>
+      <c r="H3" s="5">
+        <f>F3*G3</f>
+        <v>54.06</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="H3" s="5">
-        <v>9.01</v>
-      </c>
-      <c r="I3" s="5">
-        <f t="shared" si="0"/>
-        <v>54.06</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -791,56 +816,56 @@
       <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="8">
-        <v>6</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="7">
+        <v>6</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.27</v>
+      </c>
+      <c r="H4" s="5">
+        <f>F4*G4</f>
+        <v>7.62</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1.27</v>
-      </c>
-      <c r="I4" s="5">
-        <f t="shared" si="0"/>
-        <v>7.62</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="7">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1.08</v>
+      </c>
+      <c r="H5" s="5">
+        <f>F5*G5</f>
+        <v>6.48</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="8">
-        <v>6</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1.08</v>
-      </c>
-      <c r="I5" s="5">
-        <f t="shared" si="0"/>
-        <v>6.48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -849,58 +874,58 @@
         <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="7">
+        <v>6</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.97</v>
+      </c>
+      <c r="H6" s="5">
+        <f>F6*G6</f>
+        <v>5.82</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="8">
-        <v>6</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="I6" s="5">
-        <f t="shared" si="0"/>
-        <v>5.82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.91</v>
+      </c>
+      <c r="H7" s="5">
+        <f>F7*G7</f>
+        <v>5.46</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" s="8">
-        <v>6</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.91</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" si="0"/>
-        <v>5.46</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
@@ -909,313 +934,313 @@
         <v>10</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="7">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1.46</v>
+      </c>
+      <c r="H8" s="5">
+        <f>F8*G8</f>
+        <v>8.76</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="F8" s="8">
-        <v>6</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1.46</v>
-      </c>
-      <c r="I8" s="5">
-        <f t="shared" si="0"/>
-        <v>8.76</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="8">
-        <v>6</v>
-      </c>
-      <c r="G9" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="F9" s="7">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3.95</v>
+      </c>
       <c r="H9" s="5">
-        <v>3.95</v>
-      </c>
-      <c r="I9" s="5">
-        <f t="shared" si="0"/>
+        <f>F9*G9</f>
         <v>23.700000000000003</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="8">
-        <v>6</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="F10" s="7">
+        <v>6</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.89</v>
       </c>
       <c r="H10" s="5">
-        <v>0.89</v>
-      </c>
-      <c r="I10" s="5">
-        <f t="shared" si="0"/>
+        <f>F10*G10</f>
         <v>5.34</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" s="2">
         <v>100</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>51</v>
+      <c r="G11" s="5">
+        <v>0.219</v>
       </c>
       <c r="H11" s="5">
-        <v>0.219</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0.219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <f>G11*F11</f>
+        <v>21.9</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="2">
+        <v>6</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="H12" s="5">
+        <f>F12*G12</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="2">
+        <v>6</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.75275999999999998</v>
+      </c>
+      <c r="H13" s="5">
+        <f>F13*G13</f>
+        <v>4.5165600000000001</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="2">
-        <v>6</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="I12" s="5">
-        <f t="shared" si="0"/>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1.33</v>
+      </c>
+      <c r="H14" s="5">
+        <f>F14*G14</f>
+        <v>7.98</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="2">
-        <v>6</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.75275999999999998</v>
-      </c>
-      <c r="I13" s="5">
-        <f t="shared" si="0"/>
-        <v>4.5165600000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="2">
-        <v>6</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="5">
-        <v>1.33</v>
-      </c>
-      <c r="I14" s="5">
-        <f t="shared" si="0"/>
-        <v>7.98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>72</v>
+        <v>21</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="F15" s="2">
         <v>18</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>70</v>
+      <c r="G15" s="5">
+        <v>0.35</v>
       </c>
       <c r="H15" s="5">
-        <v>0.35</v>
-      </c>
-      <c r="I15" s="5">
-        <f t="shared" si="0"/>
+        <f>F15*G15</f>
         <v>6.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I15" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>78</v>
+        <v>31</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="F16" s="2">
         <v>6</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>77</v>
+      <c r="G16" s="5">
+        <v>0.27</v>
       </c>
       <c r="H16" s="5">
-        <v>0.27</v>
-      </c>
-      <c r="I16" s="5">
-        <f t="shared" si="0"/>
+        <f>F16*G16</f>
         <v>1.62</v>
       </c>
+      <c r="I16" s="12" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="7">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15">
+        <f>SUM(G2:G16)</f>
+        <v>30.61176</v>
+      </c>
+      <c r="H17" s="16">
         <f>SUM(H2:H16)</f>
-        <v>30.61176</v>
-      </c>
-      <c r="I17" s="5">
-        <f>SUM(I2:I16)</f>
-        <v>186.77555999999998</v>
-      </c>
+        <v>208.45656</v>
+      </c>
+      <c r="I17" s="14"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" s="13"/>
+      <c r="A19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G20" s="1"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A17:G17"/>
+  <mergeCells count="1">
     <mergeCell ref="A19:B19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId1"/>
+    <hyperlink ref="I4" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3" display="http://www.mouser.com/hiroseconnector/"/>
     <hyperlink ref="C7" r:id="rId4" display="http://digikey.com/Suppliers/us/Semtech.page?lang=en"/>
-    <hyperlink ref="G9" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="I9" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
     <hyperlink ref="C11" r:id="rId7" display="http://www.mouser.com/vishaysemiconductors/"/>
     <hyperlink ref="C12" r:id="rId8" display="http://digikey.com/Suppliers/us/Fairchild-Semiconductor.page?lang=en"/>
     <hyperlink ref="C13" r:id="rId9" display="http://digikey.com/Suppliers/us/Elna-America.page?lang=en"/>
     <hyperlink ref="C14" r:id="rId10" display="http://digikey.com/Suppliers/us/C-and-K-Components.page?lang=en"/>
     <hyperlink ref="C2" r:id="rId11" display="http://digikey.com/Suppliers/us/Analog-Devices.page?lang=en"/>
-    <hyperlink ref="G16" r:id="rId12"/>
-    <hyperlink ref="G15" r:id="rId13"/>
-    <hyperlink ref="G11" r:id="rId14"/>
-    <hyperlink ref="G2" r:id="rId15"/>
+    <hyperlink ref="I16" r:id="rId12"/>
+    <hyperlink ref="I15" r:id="rId13"/>
+    <hyperlink ref="I11" r:id="rId14"/>
+    <hyperlink ref="I2" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>

</xml_diff>